<commit_message>
added offer donwload function
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/OfferInRussian.xlsx
+++ b/src/main/resources/templates/OfferInRussian.xlsx
@@ -13,7 +13,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$14:$I$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -86,10 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,57 +117,12 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -228,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -242,57 +193,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -854,34 +778,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="7" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="20" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -912,64 +836,64 @@
       <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16"/>
@@ -1003,79 +927,290 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D20" s="11"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
improving the creation of the offer file
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/OfferInRussian.xlsx
+++ b/src/main/resources/templates/OfferInRussian.xlsx
@@ -88,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +197,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -219,15 +226,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -238,6 +236,19 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -803,7 +814,7 @@
   <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:I114"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,21 +824,25 @@
     <col min="3" max="3" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="7" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="20" style="7" customWidth="1"/>
+    <col min="6" max="6" width="23" style="7" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -861,53 +876,53 @@
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -952,773 +967,773 @@
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="7"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="7"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="7"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E47" s="7"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" s="7"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E49" s="7"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E50" s="7"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E51" s="7"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E52" s="7"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E53" s="7"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E54" s="7"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E55" s="7"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E56" s="7"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E57" s="7"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E58" s="7"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E59" s="7"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E60" s="7"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E61" s="7"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E62" s="7"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E63" s="7"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E64" s="7"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
     </row>
     <row r="65" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E65" s="7"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
     </row>
     <row r="66" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E66" s="7"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
     </row>
     <row r="67" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E67" s="7"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
     </row>
     <row r="68" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E68" s="7"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
     </row>
     <row r="69" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E69" s="7"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
     </row>
     <row r="70" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E70" s="7"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
     <row r="71" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E71" s="7"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
     <row r="72" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E72" s="7"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
     <row r="73" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E73" s="7"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
     </row>
     <row r="74" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E74" s="7"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
     <row r="75" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E75" s="7"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
     <row r="76" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E76" s="7"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
     </row>
     <row r="77" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E77" s="7"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
     </row>
     <row r="78" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E78" s="7"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
     </row>
     <row r="79" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E79" s="7"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
     <row r="80" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E80" s="7"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E81" s="7"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
     </row>
     <row r="82" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E82" s="7"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
     </row>
     <row r="83" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E83" s="7"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
     </row>
     <row r="84" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E84" s="7"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
     </row>
     <row r="85" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E85" s="7"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E86" s="7"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
     </row>
     <row r="87" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E87" s="7"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
     <row r="88" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E88" s="7"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
     </row>
     <row r="89" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E89" s="7"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
     <row r="90" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E90" s="7"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
     <row r="91" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E91" s="7"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
     <row r="92" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E92" s="7"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
     <row r="93" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E93" s="7"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
     </row>
     <row r="94" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E94" s="7"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
     <row r="95" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E95" s="7"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
     </row>
     <row r="96" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E96" s="7"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
     </row>
     <row r="97" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E97" s="7"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
     </row>
     <row r="98" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E98" s="7"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
     </row>
     <row r="99" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E99" s="7"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
     <row r="100" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E100" s="7"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
     </row>
     <row r="101" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E101" s="7"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
       <c r="I101" s="7"/>
     </row>
     <row r="102" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E102" s="7"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
       <c r="I102" s="7"/>
     </row>
     <row r="103" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E103" s="7"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
       <c r="I103" s="7"/>
     </row>
     <row r="104" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E104" s="7"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
       <c r="I104" s="7"/>
     </row>
     <row r="105" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E105" s="7"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="15"/>
       <c r="I105" s="7"/>
     </row>
     <row r="106" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E106" s="7"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
       <c r="I106" s="7"/>
     </row>
     <row r="107" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E107" s="7"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="18"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="15"/>
       <c r="I107" s="7"/>
     </row>
     <row r="108" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E108" s="7"/>
-      <c r="F108" s="18"/>
+      <c r="F108" s="15"/>
       <c r="I108" s="7"/>
     </row>
     <row r="109" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E109" s="7"/>
-      <c r="F109" s="18"/>
+      <c r="F109" s="15"/>
       <c r="I109" s="7"/>
     </row>
     <row r="110" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E110" s="7"/>
-      <c r="F110" s="18"/>
+      <c r="F110" s="15"/>
       <c r="I110" s="7"/>
     </row>
     <row r="111" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E111" s="7"/>
-      <c r="F111" s="18"/>
+      <c r="F111" s="15"/>
       <c r="I111" s="7"/>
     </row>
     <row r="112" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E112" s="7"/>
-      <c r="F112" s="18"/>
+      <c r="F112" s="15"/>
       <c r="I112" s="7"/>
     </row>
     <row r="113" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E113" s="7"/>
-      <c r="F113" s="18"/>
+      <c r="F113" s="15"/>
       <c r="I113" s="7"/>
     </row>
     <row r="114" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E114" s="7"/>
-      <c r="F114" s="18"/>
+      <c r="F114" s="15"/>
       <c r="I114" s="7"/>
     </row>
     <row r="115" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E115" s="7"/>
-      <c r="F115" s="18"/>
+      <c r="F115" s="15"/>
     </row>
     <row r="116" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F116" s="18"/>
+      <c r="F116" s="15"/>
     </row>
     <row r="117" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F117" s="18"/>
+      <c r="F117" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>